<commit_message>
added more industry tests
</commit_message>
<xml_diff>
--- a/data/steel/steel_simplified_calcs.xlsx
+++ b/data/steel/steel_simplified_calcs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setanzer\GitHub\BlackBlox\data\steel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/steel/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9E8600-E8F7-7B44-BC58-E080E0E762E4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5745" yWindow="465" windowWidth="20820" windowHeight="17535" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="5740" yWindow="460" windowWidth="20820" windowHeight="17540" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coke" sheetId="1" r:id="rId1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="154">
   <si>
     <t>combustion</t>
   </si>
@@ -93,9 +94,6 @@
     <t>steel</t>
   </si>
   <si>
-    <t>scrap</t>
-  </si>
-  <si>
     <t>coinflows</t>
   </si>
   <si>
@@ -402,9 +400,6 @@
     <t>total metal</t>
   </si>
   <si>
-    <t>hot metal demand</t>
-  </si>
-  <si>
     <t>slag__steel loss</t>
   </si>
   <si>
@@ -502,12 +497,15 @@
   </si>
   <si>
     <t>O2 demand</t>
+  </si>
+  <si>
+    <t>total metal demand</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -630,8 +628,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -942,64 +940,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>1</v>
@@ -1008,21 +1006,21 @@
         <v>9</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C3" s="17" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>2</v>
@@ -1031,15 +1029,15 @@
         <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>4</v>
@@ -1054,12 +1052,12 @@
         <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>3</v>
@@ -1068,7 +1066,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>4</v>
@@ -1077,41 +1075,41 @@
         <v>8</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B6" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="17" t="s">
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>141</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>143</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>4</v>
@@ -1120,41 +1118,41 @@
         <v>8</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="B8" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>142</v>
-      </c>
       <c r="E8" s="17" t="s">
         <v>4</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>2</v>
@@ -1163,21 +1161,21 @@
         <v>9</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>1</v>
@@ -1192,62 +1190,62 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1256,62 +1254,62 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.875" style="1"/>
+    <col min="3" max="3" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>4</v>
@@ -1320,58 +1318,58 @@
         <v>9</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>4</v>
@@ -1380,84 +1378,84 @@
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="16" t="s">
         <v>15</v>
@@ -1469,122 +1467,122 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
@@ -1596,57 +1594,57 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.625" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
@@ -1654,19 +1652,19 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
         <v>82</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>83</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1674,19 +1672,19 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" t="s">
         <v>84</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="F3" t="s">
-        <v>83</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
@@ -1700,13 +1698,13 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -1714,7 +1712,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
@@ -1723,7 +1721,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -1731,27 +1729,27 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="E6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" t="s">
-        <v>83</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
         <v>4</v>
@@ -1761,35 +1759,35 @@
       </c>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="E8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" s="11" t="s">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>93</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
@@ -1799,58 +1797,58 @@
       </c>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
       </c>
       <c r="F10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>94</v>
       </c>
-      <c r="H10" t="s">
-        <v>56</v>
-      </c>
-      <c r="I10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>82</v>
+      </c>
+      <c r="G11" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="E11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" t="s">
-        <v>83</v>
-      </c>
-      <c r="G11" s="11" t="s">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>95</v>
-      </c>
-      <c r="C12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" t="s">
-        <v>97</v>
       </c>
       <c r="E12" t="s">
         <v>1</v>
@@ -1866,195 +1864,195 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D8" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D8" t="s">
-        <v>148</v>
       </c>
       <c r="E8" t="s">
         <v>4</v>
@@ -2063,38 +2061,38 @@
         <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F9" t="s">
         <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -2103,53 +2101,53 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F10" t="s">
         <v>8</v>
       </c>
       <c r="G10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2158,105 +2156,105 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>1</v>
@@ -2265,18 +2263,18 @@
         <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
@@ -2291,24 +2289,24 @@
         <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>2</v>
@@ -2317,21 +2315,21 @@
         <v>9</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>1</v>
@@ -2340,10 +2338,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J9" s="1"/>
     </row>
   </sheetData>
@@ -2352,63 +2350,63 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
@@ -2417,21 +2415,21 @@
         <v>9</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>4</v>
@@ -2440,18 +2438,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>4</v>
@@ -2460,21 +2458,21 @@
         <v>9</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>4</v>
@@ -2483,21 +2481,21 @@
         <v>8</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>4</v>
@@ -2506,18 +2504,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>4</v>
@@ -2526,18 +2524,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>2</v>
@@ -2546,21 +2544,21 @@
         <v>9</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>2</v>
@@ -2569,21 +2567,21 @@
         <v>8</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>2</v>
@@ -2592,21 +2590,21 @@
         <v>9</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>1</v>
@@ -2621,63 +2619,63 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
@@ -2686,21 +2684,21 @@
         <v>9</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>4</v>
@@ -2709,18 +2707,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>4</v>
@@ -2729,21 +2727,21 @@
         <v>9</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>4</v>
@@ -2752,21 +2750,21 @@
         <v>8</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>4</v>
@@ -2775,18 +2773,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>4</v>
@@ -2795,18 +2793,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>2</v>
@@ -2815,21 +2813,21 @@
         <v>9</v>
       </c>
       <c r="G8" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>2</v>
@@ -2838,21 +2836,21 @@
         <v>8</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>2</v>
@@ -2861,21 +2859,21 @@
         <v>9</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>1</v>
@@ -2890,109 +2888,109 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>4</v>
@@ -3001,21 +2999,21 @@
         <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>114</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>115</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>4</v>
@@ -3024,18 +3022,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>4</v>
@@ -3044,21 +3042,21 @@
         <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>4</v>
@@ -3067,21 +3065,21 @@
         <v>8</v>
       </c>
       <c r="G7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>111</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>112</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>4</v>
@@ -3090,18 +3088,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>4</v>
@@ -3110,18 +3108,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>4</v>
@@ -3130,21 +3128,21 @@
         <v>9</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>4</v>
@@ -3153,41 +3151,41 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>4</v>
@@ -3196,86 +3194,86 @@
         <v>8</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F14" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F15" s="18" t="s">
         <v>0</v>
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="19" t="s">
         <v>1</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>2</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>2</v>
@@ -3284,21 +3282,21 @@
         <v>9</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>1</v>
@@ -3307,35 +3305,35 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>1</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>2</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>2</v>
@@ -3350,18 +3348,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>4</v>
@@ -3370,18 +3368,18 @@
         <v>5</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>4</v>
@@ -3393,10 +3391,10 @@
         <v>12</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>1</v>
@@ -3408,64 +3406,64 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>18</v>
+      <c r="D2" s="19" t="s">
+        <v>143</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
@@ -3474,98 +3472,98 @@
         <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>2</v>
+      <c r="D3" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>4</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>5</v>
+      <c r="B4" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>93</v>
       </c>
       <c r="G4" s="13"/>
-      <c r="H4" s="10" t="s">
-        <v>18</v>
+      <c r="H4" s="19" t="s">
+        <v>143</v>
       </c>
       <c r="I4" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>122</v>
-      </c>
       <c r="E5" s="10" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G5" s="13"/>
       <c r="H5" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>4</v>
@@ -3574,21 +3572,21 @@
         <v>9</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>4</v>
@@ -3597,18 +3595,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>4</v>
@@ -3617,21 +3615,21 @@
         <v>9</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>4</v>
@@ -3640,84 +3638,84 @@
         <v>8</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="E11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>36</v>
-      </c>
       <c r="G12" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>1</v>
@@ -3727,18 +3725,18 @@
       </c>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>2</v>
@@ -3747,21 +3745,21 @@
         <v>9</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>1</v>
@@ -3770,41 +3768,41 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="12" t="s">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>1</v>
@@ -3819,75 +3817,75 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
@@ -3896,7 +3894,7 @@
         <v>9</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -3904,27 +3902,27 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -3932,27 +3930,27 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -3960,21 +3958,21 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>15</v>
@@ -3986,7 +3984,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -4000,7 +3998,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4020,62 +4018,62 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.875" style="1"/>
+    <col min="3" max="3" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>4</v>
@@ -4084,27 +4082,27 @@
         <v>8</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned up Var file
</commit_message>
<xml_diff>
--- a/data/steel/steel_simplified_calcs.xlsx
+++ b/data/steel/steel_simplified_calcs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/steel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setanzer\GitHub\BlackBlox\data\steel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9E8600-E8F7-7B44-BC58-E080E0E762E4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5740" yWindow="460" windowWidth="20820" windowHeight="17540" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5745" yWindow="465" windowWidth="20820" windowHeight="17535" firstSheet="8" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Coke" sheetId="1" r:id="rId1"/>
@@ -27,6 +26,8 @@
     <sheet name="CO2 Storage" sheetId="14" r:id="rId12"/>
     <sheet name="Fuel" sheetId="11" r:id="rId13"/>
     <sheet name="EAF" sheetId="17" r:id="rId14"/>
+    <sheet name="DRI" sheetId="18" r:id="rId15"/>
+    <sheet name="electrolysis" sheetId="19" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="159">
   <si>
     <t>combustion</t>
   </si>
@@ -500,15 +501,37 @@
   </si>
   <si>
     <t>total metal demand</t>
+  </si>
+  <si>
+    <t>iron sponge</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> outflows</t>
+  </si>
+  <si>
+    <t>fuel__eq</t>
+  </si>
+  <si>
+    <t>fuel eq energy</t>
+  </si>
+  <si>
+    <t>fuel energy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -598,38 +621,39 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -940,21 +964,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -986,7 +1010,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1009,7 +1033,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1032,7 +1056,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1055,7 +1079,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>138</v>
       </c>
@@ -1078,7 +1102,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>138</v>
       </c>
@@ -1098,7 +1122,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>138</v>
       </c>
@@ -1121,7 +1145,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>138</v>
       </c>
@@ -1141,7 +1165,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
@@ -1164,7 +1188,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
@@ -1190,16 +1214,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -1228,7 +1252,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1254,25 +1278,25 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="19.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -1301,7 +1325,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>121</v>
       </c>
@@ -1324,7 +1348,7 @@
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>121</v>
       </c>
@@ -1347,7 +1371,7 @@
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>122</v>
       </c>
@@ -1367,7 +1391,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>122</v>
       </c>
@@ -1387,7 +1411,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>135</v>
       </c>
@@ -1407,7 +1431,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>20</v>
       </c>
@@ -1424,7 +1448,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>135</v>
       </c>
@@ -1444,7 +1468,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>126</v>
       </c>
@@ -1467,22 +1491,22 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -1511,7 +1535,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>135</v>
       </c>
@@ -1531,7 +1555,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>135</v>
       </c>
@@ -1551,7 +1575,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -1571,7 +1595,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1594,25 +1618,25 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>30</v>
       </c>
@@ -1644,7 +1668,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
@@ -1664,7 +1688,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
@@ -1684,7 +1708,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
@@ -1704,7 +1728,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -1721,7 +1745,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -1741,7 +1765,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>88</v>
       </c>
@@ -1759,7 +1783,7 @@
       </c>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>55</v>
       </c>
@@ -1779,7 +1803,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>90</v>
       </c>
@@ -1797,7 +1821,7 @@
       </c>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>90</v>
       </c>
@@ -1820,7 +1844,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>92</v>
       </c>
@@ -1840,7 +1864,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>94</v>
       </c>
@@ -1864,20 +1888,20 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>30</v>
       </c>
@@ -1909,7 +1933,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1932,7 +1956,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1955,7 +1979,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>121</v>
       </c>
@@ -1978,7 +2002,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>121</v>
       </c>
@@ -1998,7 +2022,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -2021,7 +2045,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>74</v>
       </c>
@@ -2041,7 +2065,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>74</v>
       </c>
@@ -2064,7 +2088,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -2087,7 +2111,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>74</v>
       </c>
@@ -2110,7 +2134,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>74</v>
       </c>
@@ -2130,7 +2154,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -2155,17 +2179,218 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="21"/>
+      <c r="B3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2197,7 +2422,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -2220,7 +2445,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
@@ -2243,7 +2468,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -2269,7 +2494,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -2295,7 +2520,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -2318,7 +2543,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -2338,10 +2563,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J9" s="1"/>
     </row>
   </sheetData>
@@ -2350,20 +2575,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2395,7 +2620,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2418,7 +2643,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2438,7 +2663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2461,7 +2686,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2484,7 +2709,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2504,7 +2729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -2524,7 +2749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>60</v>
       </c>
@@ -2547,7 +2772,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>60</v>
       </c>
@@ -2570,7 +2795,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
@@ -2593,7 +2818,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -2619,20 +2844,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2664,7 +2889,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2687,7 +2912,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2707,7 +2932,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2730,7 +2955,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2753,7 +2978,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2773,7 +2998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -2793,7 +3018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
@@ -2816,7 +3041,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>33</v>
       </c>
@@ -2839,7 +3064,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
@@ -2862,7 +3087,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -2888,20 +3113,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="A4" sqref="A4:G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -2933,7 +3158,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -2956,7 +3181,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -2979,7 +3204,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>53</v>
       </c>
@@ -3002,7 +3227,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>53</v>
       </c>
@@ -3022,7 +3247,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -3045,7 +3270,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>53</v>
       </c>
@@ -3068,7 +3293,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>53</v>
       </c>
@@ -3088,7 +3313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>53</v>
       </c>
@@ -3108,7 +3333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>151</v>
       </c>
@@ -3131,7 +3356,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>151</v>
       </c>
@@ -3151,7 +3376,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>151</v>
       </c>
@@ -3174,7 +3399,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>151</v>
       </c>
@@ -3197,7 +3422,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>151</v>
       </c>
@@ -3217,7 +3442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>151</v>
       </c>
@@ -3238,7 +3463,7 @@
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>151</v>
       </c>
@@ -3262,7 +3487,7 @@
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>20</v>
       </c>
@@ -3285,7 +3510,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
@@ -3305,7 +3530,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>11</v>
       </c>
@@ -3328,7 +3553,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>11</v>
       </c>
@@ -3348,7 +3573,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>10</v>
       </c>
@@ -3374,7 +3599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>10</v>
       </c>
@@ -3406,21 +3631,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
@@ -3452,7 +3677,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -3475,7 +3700,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -3498,7 +3723,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>17</v>
       </c>
@@ -3525,7 +3750,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>17</v>
       </c>
@@ -3552,7 +3777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>65</v>
       </c>
@@ -3575,7 +3800,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>65</v>
       </c>
@@ -3595,7 +3820,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>65</v>
       </c>
@@ -3618,7 +3843,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>65</v>
       </c>
@@ -3641,7 +3866,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>65</v>
       </c>
@@ -3661,7 +3886,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>65</v>
       </c>
@@ -3681,7 +3906,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>11</v>
       </c>
@@ -3704,7 +3929,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
@@ -3725,7 +3950,7 @@
       </c>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
@@ -3748,7 +3973,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
@@ -3768,7 +3993,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>97</v>
       </c>
@@ -3791,7 +4016,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>97</v>
       </c>
@@ -3817,30 +4042,30 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>30</v>
       </c>
@@ -3874,7 +4099,7 @@
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>77</v>
       </c>
@@ -3902,7 +4127,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>77</v>
       </c>
@@ -3930,7 +4155,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>74</v>
       </c>
@@ -3958,7 +4183,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>74</v>
       </c>
@@ -3984,7 +4209,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -3998,7 +4223,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -4018,25 +4243,25 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="17.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -4065,7 +4290,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>20</v>
       </c>
@@ -4085,7 +4310,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
added DRI process to calcs file
</commit_message>
<xml_diff>
--- a/data/steel/steel_simplified_calcs.xlsx
+++ b/data/steel/steel_simplified_calcs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5745" yWindow="465" windowWidth="20820" windowHeight="17535" firstSheet="8" activeTab="13"/>
+    <workbookView xWindow="5745" yWindow="465" windowWidth="20820" windowHeight="17535" firstSheet="8" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Coke" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,9 @@
     <sheet name="CO2 Capture" sheetId="13" r:id="rId11"/>
     <sheet name="CO2 Storage" sheetId="14" r:id="rId12"/>
     <sheet name="Fuel" sheetId="11" r:id="rId13"/>
-    <sheet name="EAF" sheetId="17" r:id="rId14"/>
-    <sheet name="DRI" sheetId="18" r:id="rId15"/>
-    <sheet name="electrolysis" sheetId="19" r:id="rId16"/>
+    <sheet name="Ore" sheetId="20" r:id="rId14"/>
+    <sheet name="EAF" sheetId="17" r:id="rId15"/>
+    <sheet name="DRI" sheetId="18" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1634,8 +1634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1902,9 +1902,21 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -2192,7 +2204,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
@@ -2354,20 +2366,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
started process for charcoal
</commit_message>
<xml_diff>
--- a/data/steel/steel_simplified_calcs.xlsx
+++ b/data/steel/steel_simplified_calcs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/steel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setanzer\GitHub\BlackBlox\data\steel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA077EA-3BD1-514E-ABBD-C0721C3A42ED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6100" yWindow="460" windowWidth="21380" windowHeight="17540" firstSheet="2" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6105" yWindow="465" windowWidth="21375" windowHeight="17535" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Coke" sheetId="1" r:id="rId1"/>
@@ -20,14 +19,15 @@
     <sheet name="Iron" sheetId="8" r:id="rId5"/>
     <sheet name="Steel" sheetId="3" r:id="rId6"/>
     <sheet name="Finish" sheetId="12" r:id="rId7"/>
-    <sheet name="DRI" sheetId="18" r:id="rId8"/>
-    <sheet name="EAF" sheetId="17" r:id="rId9"/>
-    <sheet name="Syngas" sheetId="21" r:id="rId10"/>
-    <sheet name="Oxygen" sheetId="9" r:id="rId11"/>
-    <sheet name="Electricity" sheetId="10" r:id="rId12"/>
-    <sheet name="Heat" sheetId="16" r:id="rId13"/>
-    <sheet name="CO2 Capture" sheetId="13" r:id="rId14"/>
-    <sheet name="CO2 Storage" sheetId="14" r:id="rId15"/>
+    <sheet name="Charcoal" sheetId="22" r:id="rId8"/>
+    <sheet name="DRI" sheetId="18" r:id="rId9"/>
+    <sheet name="EAF" sheetId="17" r:id="rId10"/>
+    <sheet name="Syngas" sheetId="21" r:id="rId11"/>
+    <sheet name="Oxygen" sheetId="9" r:id="rId12"/>
+    <sheet name="Electricity" sheetId="10" r:id="rId13"/>
+    <sheet name="Heat" sheetId="16" r:id="rId14"/>
+    <sheet name="CO2 Capture" sheetId="13" r:id="rId15"/>
+    <sheet name="CO2 Storage" sheetId="14" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="194">
   <si>
     <t>combustion</t>
   </si>
@@ -626,7 +626,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -815,8 +815,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1127,21 +1127,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>121</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>121</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>121</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>121</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>179</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>179</v>
       </c>
@@ -1417,20 +1417,460 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="E3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="I5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D12" t="s">
+        <v>129</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E15" t="s">
+        <v>116</v>
+      </c>
+      <c r="F15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" t="s">
+        <v>131</v>
+      </c>
+      <c r="E16" t="s">
+        <v>116</v>
+      </c>
+      <c r="F16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" t="s">
+        <v>116</v>
+      </c>
+      <c r="F18" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>189</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B20" t="s">
+        <v>189</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.625" customWidth="1"/>
+    <col min="4" max="4" width="19.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -1462,7 +1902,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>145</v>
       </c>
@@ -1488,7 +1928,7 @@
       <c r="I2" s="22"/>
       <c r="J2" s="22"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1512,7 +1952,7 @@
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="21" t="s">
         <v>141</v>
@@ -1534,7 +1974,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="21" t="s">
         <v>141</v>
@@ -1556,7 +1996,7 @@
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="10" t="s">
         <v>93</v>
@@ -1576,7 +2016,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="10" t="s">
         <v>54</v>
@@ -1596,7 +2036,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
@@ -1619,7 +2059,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
         <v>19</v>
       </c>
@@ -1636,7 +2076,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>73</v>
       </c>
@@ -1659,7 +2099,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>167</v>
       </c>
@@ -1682,7 +2122,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>170</v>
       </c>
@@ -1705,7 +2145,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>106</v>
       </c>
@@ -1728,7 +2168,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="22" t="s">
         <v>144</v>
       </c>
@@ -1748,7 +2188,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>150</v>
       </c>
@@ -1771,7 +2211,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="23"/>
       <c r="B16" s="28" t="s">
         <v>177</v>
@@ -1790,7 +2230,7 @@
       </c>
       <c r="G16" s="23"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>146</v>
       </c>
@@ -1816,7 +2256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" s="24" t="s">
         <v>144</v>
       </c>
@@ -1833,7 +2273,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19" s="24" t="s">
         <v>159</v>
       </c>
@@ -1856,7 +2296,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B20" s="24" t="s">
         <v>73</v>
       </c>
@@ -1879,7 +2319,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>172</v>
       </c>
@@ -1902,7 +2342,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>173</v>
       </c>
@@ -1925,7 +2365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23" s="22" t="s">
         <v>162</v>
       </c>
@@ -1948,7 +2388,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>179</v>
       </c>
@@ -1968,7 +2408,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>179</v>
       </c>
@@ -1993,17 +2433,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -2037,7 +2477,7 @@
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>75</v>
       </c>
@@ -2065,7 +2505,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>75</v>
       </c>
@@ -2093,7 +2533,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>72</v>
       </c>
@@ -2121,7 +2561,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>72</v>
       </c>
@@ -2147,7 +2587,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>179</v>
       </c>
@@ -2173,7 +2613,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>179</v>
       </c>
@@ -2204,27 +2644,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="1"/>
+    <col min="2" max="2" width="11.375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="1"/>
+    <col min="4" max="4" width="17.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -2256,7 +2696,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
         <v>19</v>
       </c>
@@ -2276,7 +2716,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2296,7 +2736,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>19</v>
       </c>
@@ -2316,7 +2756,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>179</v>
       </c>
@@ -2336,7 +2776,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>179</v>
       </c>
@@ -2347,157 +2787,6 @@
         <v>2</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>182</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="31" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:J6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>193</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B6" t="s">
-        <v>193</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="31" t="s">
         <v>182</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -2513,26 +2802,177 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" t="s">
+        <v>193</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12:F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="1"/>
+    <col min="2" max="2" width="11.375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="1"/>
+    <col min="4" max="4" width="19.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -2564,7 +3004,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>106</v>
       </c>
@@ -2590,7 +3030,7 @@
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>106</v>
       </c>
@@ -2613,7 +3053,7 @@
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>107</v>
       </c>
@@ -2633,7 +3073,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
         <v>107</v>
       </c>
@@ -2653,7 +3093,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="s">
         <v>119</v>
       </c>
@@ -2673,7 +3113,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>72</v>
       </c>
@@ -2693,7 +3133,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
         <v>119</v>
       </c>
@@ -2713,7 +3153,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>111</v>
       </c>
@@ -2730,7 +3170,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>150</v>
       </c>
@@ -2753,7 +3193,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="23"/>
       <c r="B11" s="28" t="s">
         <v>177</v>
@@ -2777,23 +3217,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -2825,7 +3265,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="s">
         <v>119</v>
       </c>
@@ -2845,7 +3285,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
         <v>119</v>
       </c>
@@ -2865,7 +3305,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>156</v>
       </c>
@@ -2885,7 +3325,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -2902,7 +3342,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>119</v>
       </c>
@@ -2922,7 +3362,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>175</v>
       </c>
@@ -2939,7 +3379,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>156</v>
       </c>
@@ -2965,16 +3405,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -3006,7 +3446,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
@@ -3029,7 +3469,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
@@ -3052,7 +3492,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -3078,7 +3518,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -3104,7 +3544,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
@@ -3127,7 +3567,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -3147,7 +3587,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>179</v>
       </c>
@@ -3168,7 +3608,7 @@
       </c>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>179</v>
       </c>
@@ -3195,20 +3635,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -3240,7 +3680,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -3263,7 +3703,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -3283,7 +3723,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -3306,7 +3746,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -3329,7 +3769,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3349,7 +3789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -3369,7 +3809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>59</v>
       </c>
@@ -3392,7 +3832,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>59</v>
       </c>
@@ -3415,7 +3855,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -3438,7 +3878,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -3458,7 +3898,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>179</v>
       </c>
@@ -3478,7 +3918,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>179</v>
       </c>
@@ -3504,20 +3944,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -3549,7 +3989,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -3572,7 +4012,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -3592,7 +4032,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -3615,7 +4055,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -3638,7 +4078,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -3658,7 +4098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -3678,7 +4118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>32</v>
       </c>
@@ -3701,7 +4141,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>32</v>
       </c>
@@ -3724,7 +4164,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
@@ -3747,7 +4187,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -3767,7 +4207,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>179</v>
       </c>
@@ -3787,7 +4227,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>179</v>
       </c>
@@ -3813,20 +4253,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -3858,7 +4298,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -3881,7 +4321,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
@@ -3904,7 +4344,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>52</v>
       </c>
@@ -3927,7 +4367,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>52</v>
       </c>
@@ -3947,7 +4387,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>52</v>
       </c>
@@ -3970,7 +4410,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>52</v>
       </c>
@@ -3993,7 +4433,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>52</v>
       </c>
@@ -4013,7 +4453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>52</v>
       </c>
@@ -4033,7 +4473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>132</v>
       </c>
@@ -4056,7 +4496,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>132</v>
       </c>
@@ -4076,7 +4516,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>132</v>
       </c>
@@ -4099,7 +4539,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>132</v>
       </c>
@@ -4122,7 +4562,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>132</v>
       </c>
@@ -4142,7 +4582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>132</v>
       </c>
@@ -4163,7 +4603,7 @@
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>132</v>
       </c>
@@ -4187,7 +4627,7 @@
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
@@ -4210,7 +4650,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>19</v>
       </c>
@@ -4230,7 +4670,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>10</v>
       </c>
@@ -4253,7 +4693,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>10</v>
       </c>
@@ -4273,7 +4713,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>9</v>
       </c>
@@ -4299,7 +4739,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>9</v>
       </c>
@@ -4325,7 +4765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>179</v>
       </c>
@@ -4345,7 +4785,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>179</v>
       </c>
@@ -4371,21 +4811,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -4417,7 +4857,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -4440,7 +4880,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -4463,7 +4903,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>16</v>
       </c>
@@ -4490,7 +4930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>16</v>
       </c>
@@ -4517,7 +4957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>64</v>
       </c>
@@ -4540,7 +4980,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>64</v>
       </c>
@@ -4560,7 +5000,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>64</v>
       </c>
@@ -4583,7 +5023,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>64</v>
       </c>
@@ -4606,7 +5046,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>64</v>
       </c>
@@ -4626,7 +5066,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>64</v>
       </c>
@@ -4646,7 +5086,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>10</v>
       </c>
@@ -4669,7 +5109,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
@@ -4690,7 +5130,7 @@
       </c>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -4713,7 +5153,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
@@ -4733,7 +5173,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>82</v>
       </c>
@@ -4756,7 +5196,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>82</v>
       </c>
@@ -4776,7 +5216,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>179</v>
       </c>
@@ -4796,7 +5236,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>179</v>
       </c>
@@ -4822,16 +5262,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -4854,7 +5294,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>16</v>
       </c>
@@ -4877,7 +5317,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="22" t="s">
         <v>33</v>
@@ -4898,7 +5338,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="27" t="s">
         <v>147</v>
@@ -4917,7 +5357,7 @@
       </c>
       <c r="G4" s="22"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="27" t="s">
         <v>176</v>
@@ -4936,7 +5376,7 @@
       </c>
       <c r="G5" s="22"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -4959,7 +5399,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
         <v>19</v>
       </c>
@@ -4976,7 +5416,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>73</v>
       </c>
@@ -4999,7 +5439,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
         <v>73</v>
       </c>
@@ -5016,7 +5456,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>10</v>
       </c>
@@ -5039,7 +5479,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
         <v>38</v>
@@ -5058,7 +5498,7 @@
       </c>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>179</v>
       </c>
@@ -5078,7 +5518,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>179</v>
       </c>
@@ -5104,20 +5544,58 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.625" customWidth="1"/>
+    <col min="4" max="4" width="22.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>29</v>
       </c>
@@ -5149,7 +5627,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>139</v>
       </c>
@@ -5172,7 +5650,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
         <v>155</v>
       </c>
@@ -5192,7 +5670,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="22" t="s">
         <v>19</v>
       </c>
@@ -5209,7 +5687,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -5232,7 +5710,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="s">
         <v>73</v>
       </c>
@@ -5249,7 +5727,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -5272,7 +5750,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -5295,7 +5773,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -5318,7 +5796,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -5338,7 +5816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
@@ -5358,7 +5836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>142</v>
       </c>
@@ -5384,7 +5862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>179</v>
       </c>
@@ -5404,7 +5882,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>179</v>
       </c>
@@ -5428,444 +5906,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:J20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="E3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" t="s">
-        <v>104</v>
-      </c>
-      <c r="E5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="I5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>138</v>
-      </c>
-      <c r="E6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>138</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" t="s">
-        <v>116</v>
-      </c>
-      <c r="F7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H7" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>106</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>125</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>116</v>
-      </c>
-      <c r="F8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>116</v>
-      </c>
-      <c r="D9" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" t="s">
-        <v>125</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F11" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>116</v>
-      </c>
-      <c r="D12" t="s">
-        <v>129</v>
-      </c>
-      <c r="E12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>129</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" t="s">
-        <v>79</v>
-      </c>
-      <c r="F13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>129</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" t="s">
-        <v>78</v>
-      </c>
-      <c r="F14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15" t="s">
-        <v>130</v>
-      </c>
-      <c r="E15" t="s">
-        <v>116</v>
-      </c>
-      <c r="F15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" t="s">
-        <v>131</v>
-      </c>
-      <c r="E16" t="s">
-        <v>116</v>
-      </c>
-      <c r="F16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" t="s">
-        <v>116</v>
-      </c>
-      <c r="D17" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" t="s">
-        <v>79</v>
-      </c>
-      <c r="F17" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" t="s">
-        <v>84</v>
-      </c>
-      <c r="E18" t="s">
-        <v>116</v>
-      </c>
-      <c r="F18" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>189</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" s="31" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="B20" t="s">
-        <v>189</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="31" t="s">
-        <v>182</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" s="31" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>